<commit_message>
cov: add preview params
</commit_message>
<xml_diff>
--- a/tests/fixtures/fixture-single-sheet.xlsx
+++ b/tests/fixtures/fixture-single-sheet.xlsx
@@ -148,13 +148,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.85"/>
@@ -177,6 +177,14 @@
         <v>2019</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>2020</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>